<commit_message>
update hardware designs for plus and protohat
update hardware designs for plus and protohat
</commit_message>
<xml_diff>
--- a/hardware/pi-crust-protohat/Pi_Crust_ProtoHAT_v1.0_Parts_List.xlsx
+++ b/hardware/pi-crust-protohat/Pi_Crust_ProtoHAT_v1.0_Parts_List.xlsx
@@ -166,7 +166,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -176,6 +176,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="29.57"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">

</xml_diff>